<commit_message>
add plot to gradient
</commit_message>
<xml_diff>
--- a/data/dashboard_overzicht.xlsx
+++ b/data/dashboard_overzicht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kco_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1864CD9-571F-864F-B348-3BE5D1FC630B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65F6AC6-3B4E-4340-BAEE-919A22A78E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33620" yWindow="-1300" windowWidth="28800" windowHeight="17500" xr2:uid="{6DCFAA71-C545-9047-BBA0-2A62278492E6}"/>
+    <workbookView xWindow="-33620" yWindow="-1300" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{6DCFAA71-C545-9047-BBA0-2A62278492E6}"/>
   </bookViews>
   <sheets>
     <sheet name="uitkomst" sheetId="1" r:id="rId1"/>
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="143">
   <si>
     <t>Laag geboortegewicht</t>
   </si>
@@ -575,15 +575,6 @@
     <t>uitkomstmaat</t>
   </si>
   <si>
-    <t>Metropoolregio</t>
-  </si>
-  <si>
-    <t>Stadsdelen</t>
-  </si>
-  <si>
-    <t>Gebieden</t>
-  </si>
-  <si>
     <t>Ontvanger van bijstandsuitkering.</t>
   </si>
   <si>
@@ -660,6 +651,12 @@
   </si>
   <si>
     <t>1984-1987</t>
+  </si>
+  <si>
+    <t>Stadsdeel Amsterdam</t>
+  </si>
+  <si>
+    <t>Gebied Amsterdam</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FAA6C8-DA36-8C43-9A13-1D27FEB3367E}">
   <dimension ref="A1:W990"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -1106,7 +1103,7 @@
         <v>112</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>113</v>
@@ -1136,13 +1133,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1169,10 +1166,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>2</v>
@@ -1202,10 +1199,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>4</v>
@@ -1235,13 +1232,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1268,13 +1265,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1301,13 +1298,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1334,13 +1331,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1367,10 +1364,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>10</v>
@@ -1400,10 +1397,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>12</v>
@@ -1433,13 +1430,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1466,13 +1463,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1499,10 +1496,10 @@
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>16</v>
@@ -1532,10 +1529,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>18</v>
@@ -1565,10 +1562,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>20</v>
@@ -1601,10 +1598,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1634,7 +1631,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>24</v>
@@ -1667,7 +1664,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>26</v>
@@ -1697,10 +1694,10 @@
         <v>27</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>28</v>
@@ -1730,10 +1727,10 @@
         <v>29</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>30</v>
@@ -1763,10 +1760,10 @@
         <v>31</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>32</v>
@@ -1796,13 +1793,13 @@
         <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1829,13 +1826,13 @@
         <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1862,13 +1859,13 @@
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1895,13 +1892,13 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1928,13 +1925,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1961,13 +1958,13 @@
         <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1994,10 +1991,10 @@
         <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>40</v>
@@ -2027,10 +2024,10 @@
         <v>41</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>42</v>
@@ -2060,10 +2057,10 @@
         <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>44</v>
@@ -2093,10 +2090,10 @@
         <v>45</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>46</v>
@@ -2126,10 +2123,10 @@
         <v>47</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>48</v>
@@ -26114,8 +26111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3D01D6-41A9-E04F-A986-C647638292EB}">
   <dimension ref="A1:W142"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26127,15 +26124,15 @@
   <sheetData>
     <row r="1" spans="1:23" ht="11" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>49</v>
@@ -26164,7 +26161,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>50</v>
@@ -26193,7 +26190,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>51</v>
@@ -26222,7 +26219,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>52</v>
@@ -26230,7 +26227,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>53</v>
@@ -26238,7 +26235,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>54</v>
@@ -26246,7 +26243,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>55</v>
@@ -26254,7 +26251,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>56</v>
@@ -26262,7 +26259,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>57</v>
@@ -26270,7 +26267,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>58</v>
@@ -26278,7 +26275,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>59</v>
@@ -26286,7 +26283,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>60</v>
@@ -26294,7 +26291,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>61</v>
@@ -26302,7 +26299,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>62</v>
@@ -26310,7 +26307,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>63</v>
@@ -26318,7 +26315,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>64</v>
@@ -26326,7 +26323,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>65</v>
@@ -26334,7 +26331,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>66</v>
@@ -26342,7 +26339,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>67</v>
@@ -26350,7 +26347,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>68</v>
@@ -26358,7 +26355,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>69</v>
@@ -26366,7 +26363,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>70</v>
@@ -26374,7 +26371,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>71</v>
@@ -26382,7 +26379,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>72</v>
@@ -26390,7 +26387,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>73</v>
@@ -26398,7 +26395,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>74</v>
@@ -26406,7 +26403,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>75</v>
@@ -26414,7 +26411,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>76</v>
@@ -26422,7 +26419,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>77</v>
@@ -26430,7 +26427,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>78</v>
@@ -26438,7 +26435,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>79</v>
@@ -26446,7 +26443,7 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>80</v>
@@ -26454,7 +26451,7 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>81</v>
@@ -26462,7 +26459,7 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>82</v>
@@ -26470,7 +26467,7 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>83</v>
@@ -26499,7 +26496,7 @@
     </row>
     <row r="37" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>84</v>
@@ -26507,7 +26504,7 @@
     </row>
     <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>85</v>
@@ -26515,7 +26512,7 @@
     </row>
     <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>86</v>
@@ -26523,7 +26520,7 @@
     </row>
     <row r="40" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>87</v>
@@ -26531,7 +26528,7 @@
     </row>
     <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>88</v>
@@ -26539,7 +26536,7 @@
     </row>
     <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>89</v>
@@ -26547,7 +26544,7 @@
     </row>
     <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>90</v>
@@ -26576,7 +26573,7 @@
     </row>
     <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>91</v>
@@ -26584,7 +26581,7 @@
     </row>
     <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>92</v>
@@ -26592,7 +26589,7 @@
     </row>
     <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>93</v>
@@ -26600,7 +26597,7 @@
     </row>
     <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>94</v>
@@ -26608,15 +26605,15 @@
     </row>
     <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>95</v>
@@ -26624,7 +26621,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>96</v>
@@ -26632,7 +26629,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>97</v>
@@ -26640,7 +26637,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>98</v>
@@ -26648,7 +26645,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>99</v>
@@ -26656,7 +26653,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>100</v>
@@ -26664,7 +26661,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>101</v>
@@ -26672,7 +26669,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>102</v>
@@ -26680,7 +26677,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>103</v>
@@ -26688,7 +26685,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>104</v>
@@ -26696,7 +26693,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>105</v>
@@ -26704,7 +26701,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>106</v>
@@ -26712,7 +26709,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>107</v>
@@ -26720,7 +26717,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>108</v>
@@ -26728,7 +26725,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>109</v>
@@ -26736,7 +26733,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>110</v>
@@ -26744,7 +26741,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>111</v>

</xml_diff>